<commit_message>
Update Service With Responses
</commit_message>
<xml_diff>
--- a/1.MockServices/5.TCP-IP/ATPActivationSystemPlainTextContract.xlsx
+++ b/1.MockServices/5.TCP-IP/ATPActivationSystemPlainTextContract.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco.caipe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco.caipe\Documents\Github\SOA_PICA\soa_pica\1.MockServices\5.TCP-IP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A53B3A1-E8F3-41E1-8BFE-846BC1C11949}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F6E33DE-662E-4784-80FB-26382D6F9386}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="0" windowWidth="22092" windowHeight="9660" activeTab="1" xr2:uid="{A79B9A2D-2B00-4CEF-B989-35EDED376E6C}"/>
+    <workbookView xWindow="1896" yWindow="0" windowWidth="22092" windowHeight="9660" activeTab="2" xr2:uid="{A79B9A2D-2B00-4CEF-B989-35EDED376E6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Activar" sheetId="1" r:id="rId1"/>
     <sheet name="Cancelar" sheetId="2" r:id="rId2"/>
+    <sheet name="Response" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>Posicion del campo</t>
   </si>
@@ -71,6 +72,33 @@
   </si>
   <si>
     <t>Valor Operacion</t>
+  </si>
+  <si>
+    <t>CodigoRespuesta</t>
+  </si>
+  <si>
+    <t>Mensaje</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>Activacion Exitosa</t>
+  </si>
+  <si>
+    <t>Cancelacion Exitosa</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>Operación desconocida</t>
   </si>
 </sst>
 </file>
@@ -114,12 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13336959-C90E-4CCC-9885-757892F0E6DD}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,4 +665,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015433CD-7468-423A-A16A-3777BC53C67D}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>